<commit_message>
Updated code and testdata
</commit_message>
<xml_diff>
--- a/AutomatedTest/TestData/Temenos/AddVerifyRemoveApplicant.xlsx
+++ b/AutomatedTest/TestData/Temenos/AddVerifyRemoveApplicant.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C8A466-DCAD-45BD-989B-E7BB9BF6455C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F70D62F-4111-41C1-8968-BF8A538710B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="101">
   <si>
     <t>TestScriptName</t>
   </si>
@@ -280,6 +280,54 @@
   </si>
   <si>
     <t>Are you a US citizen?</t>
+  </si>
+  <si>
+    <t>PercentageInclude</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Limit</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>LiabilityAccountNumber</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>15000.00</t>
+  </si>
+  <si>
+    <t>10000.00</t>
+  </si>
+  <si>
+    <t>550.00</t>
+  </si>
+  <si>
+    <t>100100-2</t>
+  </si>
+  <si>
+    <t>Medical</t>
+  </si>
+  <si>
+    <t>Collection</t>
   </si>
 </sst>
 </file>
@@ -403,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -452,9 +500,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AQ3"/>
+  <dimension ref="A1:BA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AQ1" sqref="AQ1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,7 +1020,7 @@
     <col min="6" max="16384" width="31.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="7" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" s="7" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1027,86 +1072,116 @@
       <c r="Q1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AD1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AE1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AF1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AG1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AH1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AI1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AJ1" s="7" t="s">
+      <c r="AJ1" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="AK1" s="7" t="s">
+      <c r="AK1" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AL1" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AM1" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AN1" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="AO1" s="7" t="s">
+      <c r="AO1" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AP1" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="AQ1" s="7" t="s">
+      <c r="AQ1" s="13" t="s">
         <v>81</v>
       </c>
+      <c r="AR1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT1" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU1" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AW1" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="AY1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="AZ1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="BA1" s="13" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="14" t="s">
         <v>8</v>
@@ -1126,10 +1201,44 @@
       <c r="O2" s="14"/>
       <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
-      <c r="Y2" s="19"/>
-      <c r="AH2" s="19"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
+      <c r="AP2" s="14"/>
+      <c r="AQ2" s="14"/>
+      <c r="AR2" s="14"/>
+      <c r="AS2" s="14"/>
+      <c r="AT2" s="14"/>
+      <c r="AU2" s="14"/>
+      <c r="AV2" s="14"/>
+      <c r="AW2" s="14"/>
+      <c r="AX2" s="14"/>
+      <c r="AY2" s="14"/>
+      <c r="AZ2" s="14"/>
+      <c r="BA2" s="14"/>
     </row>
-    <row r="3" spans="1:43" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>23</v>
       </c>
@@ -1258,6 +1367,36 @@
       </c>
       <c r="AQ3" s="11" t="s">
         <v>72</v>
+      </c>
+      <c r="AR3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="AS3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AT3" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="AU3" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV3" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AW3" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AX3" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="AY3" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="AZ3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="BA3" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>